<commit_message>
[Update] Mob.xlsx & Mob.csv
[Update] Mob.xlsx & Mob.csv
</commit_message>
<xml_diff>
--- a/Documents/Files/Mob.xlsx
+++ b/Documents/Files/Mob.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0DB87F-2762-4D59-8B74-078D296324AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E65946-079E-438C-BBF1-D410ABCCD731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-90" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -109,14 +109,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2200|2101|-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2200|2100|-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>달 늑대</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -174,6 +166,14 @@
   </si>
   <si>
     <t>2002|2003|2004|2100</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2101|-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2100|-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -502,7 +502,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -513,7 +513,7 @@
     <col min="5" max="9" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2">
         <v>3</v>
@@ -611,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2">
         <v>5</v>
@@ -640,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2">
         <v>8</v>
@@ -669,7 +669,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2">
         <v>12</v>
@@ -698,7 +698,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2">
         <v>12</v>
@@ -756,7 +756,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -785,7 +785,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2">
         <v>6</v>
@@ -814,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
@@ -837,13 +837,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
         <v>13</v>
@@ -866,13 +866,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2">
         <v>13</v>
@@ -895,13 +895,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2">
         <v>16</v>
@@ -924,13 +924,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2">
         <v>18</v>
@@ -953,13 +953,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2">
         <v>25</v>

</xml_diff>